<commit_message>
Added (and changed) input files for tests
</commit_message>
<xml_diff>
--- a/tests/testdata/inputfiles/configuration_2.xlsx
+++ b/tests/testdata/inputfiles/configuration_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GaussianPlume\tests\testdata\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562BC23D-03A4-45C3-8BF2-E6562E6F2459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81570C9A-64CB-42BC-B16E-4658F777B361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{72E806E7-A48D-4CBB-AA7B-38F46B3F2219}"/>
   </bookViews>
@@ -34,20 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>roughness</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>windspeed</t>
-  </si>
-  <si>
-    <t>stack height</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -69,10 +60,49 @@
     <t>TNO N77</t>
   </si>
   <si>
-    <t>measurement data</t>
-  </si>
-  <si>
     <t>C:\Python\GaussianPlume\tests\testdata\inputfiles\data_peaksonly_1.csv</t>
+  </si>
+  <si>
+    <t>qs</t>
+  </si>
+  <si>
+    <t>wind_speed</t>
+  </si>
+  <si>
+    <t>wind_direction</t>
+  </si>
+  <si>
+    <t>dx</t>
+  </si>
+  <si>
+    <t>dy</t>
+  </si>
+  <si>
+    <t>z0</t>
+  </si>
+  <si>
+    <t>zr</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>hm</t>
+  </si>
+  <si>
+    <t>molecular_mass</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>nogepa</t>
+  </si>
+  <si>
+    <t>stability_class</t>
+  </si>
+  <si>
+    <t>measurement_data_path_and_filename</t>
   </si>
 </sst>
 </file>
@@ -108,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,52 +456,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BB1CA2-2AF7-4AB3-B4AF-69F8B7888253}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -493,13 +593,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -515,7 +615,7 @@
         <v>43314.402777777781</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -534,7 +634,7 @@
         <v>43314.473611111112</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,7 +642,7 @@
         <v>43314.517361111109</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>16</v>

</xml_diff>